<commit_message>
Added VJIT properly along with "empty_cols"in json
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/VJIT/VJIT_placements.xlsx
+++ b/Files/college_info/all_colleges/VJIT/VJIT_placements.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\self\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\github\python_project-dataset\Files\college_info\all_colleges\VJIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3E5118-F6C2-4869-8C04-EDB06BF67883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B7197D-6E23-4B2A-8D5A-9DC2D444EF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$D$65</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Kaar Technologies</t>
   </si>
@@ -57,21 +60,12 @@
     <t>Zee Media</t>
   </si>
   <si>
-    <t>Virtusa</t>
-  </si>
-  <si>
     <t>Virtusa Neural Hack</t>
   </si>
   <si>
-    <t>ValueLabs</t>
-  </si>
-  <si>
     <t>Techigai</t>
   </si>
   <si>
-    <t>Capgemini</t>
-  </si>
-  <si>
     <t>ACS Solutions</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>Mphasis</t>
   </si>
   <si>
-    <t>Accenture</t>
-  </si>
-  <si>
-    <t>Quest Global</t>
-  </si>
-  <si>
     <t>Wipro</t>
   </si>
   <si>
@@ -114,12 +102,6 @@
     <t>Epam</t>
   </si>
   <si>
-    <t>Byjus</t>
-  </si>
-  <si>
-    <t>HCL</t>
-  </si>
-  <si>
     <t>TCS</t>
   </si>
   <si>
@@ -138,18 +120,12 @@
     <t>Qspiders</t>
   </si>
   <si>
-    <t>Cognizant</t>
-  </si>
-  <si>
     <t>UST Global</t>
   </si>
   <si>
     <t>Technip</t>
   </si>
   <si>
-    <t>Vistex</t>
-  </si>
-  <si>
     <t>L&amp;T</t>
   </si>
   <si>
@@ -177,9 +153,6 @@
     <t>Cadsys</t>
   </si>
   <si>
-    <t>Infosys</t>
-  </si>
-  <si>
     <t>Rexnord</t>
   </si>
   <si>
@@ -190,6 +163,75 @@
   </si>
   <si>
     <t>NTT DATA</t>
+  </si>
+  <si>
+    <t>Accenture_6.7</t>
+  </si>
+  <si>
+    <t>Accenture_4.5</t>
+  </si>
+  <si>
+    <t>Byjus_15</t>
+  </si>
+  <si>
+    <t>Byjus_6</t>
+  </si>
+  <si>
+    <t>Capgemini_4</t>
+  </si>
+  <si>
+    <t>Capgemini_7.5</t>
+  </si>
+  <si>
+    <t>Cognizant_4</t>
+  </si>
+  <si>
+    <t>Cognizant_6.75</t>
+  </si>
+  <si>
+    <t>HCL_3.65</t>
+  </si>
+  <si>
+    <t>HCL_4.25</t>
+  </si>
+  <si>
+    <t>Infosys_3.6</t>
+  </si>
+  <si>
+    <t>Infosys_5</t>
+  </si>
+  <si>
+    <t>Quest Global_3.5</t>
+  </si>
+  <si>
+    <t>Quest Global_3.25</t>
+  </si>
+  <si>
+    <t>Quest Global_3</t>
+  </si>
+  <si>
+    <t>ValueLabs_15</t>
+  </si>
+  <si>
+    <t>ValueLabs_16</t>
+  </si>
+  <si>
+    <t>Virtusa_6</t>
+  </si>
+  <si>
+    <t>Virtusa_5.5</t>
+  </si>
+  <si>
+    <t>Virtusa_4</t>
+  </si>
+  <si>
+    <t>Virtusa_6.5</t>
+  </si>
+  <si>
+    <t>Vistex_4</t>
+  </si>
+  <si>
+    <t>Vistex_4.5</t>
   </si>
 </sst>
 </file>
@@ -518,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>6.7</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -575,13 +617,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>5.5</v>
+        <v>5.16</v>
       </c>
       <c r="D5">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>1.2</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,13 +659,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>6.5</v>
+        <v>5.16</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -631,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C8">
-        <v>6.5</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,13 +687,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,13 +701,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>16</v>
+        <v>3.4</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,13 +715,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,13 +729,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="D12">
-        <v>122</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,13 +743,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,13 +757,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C14">
-        <v>5.16</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>43</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,13 +771,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C15">
-        <v>5.16</v>
+        <v>6.75</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +785,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,13 +799,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C17">
-        <v>2.2000000000000002</v>
+        <v>3.5</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +813,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="D18">
-        <v>76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,13 +827,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="D19">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,13 +841,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +855,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,13 +869,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,13 +883,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,13 +897,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C24">
-        <v>3.5</v>
+        <v>3.65</v>
       </c>
       <c r="D24">
-        <v>194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,13 +911,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C25">
-        <v>6.89</v>
+        <v>4.25</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,13 +925,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,13 +939,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C27">
-        <v>1.2</v>
+        <v>4.5</v>
       </c>
       <c r="D27">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,13 +953,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,13 +967,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C29">
-        <v>15</v>
+        <v>3.6</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,10 +981,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C30">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -953,13 +995,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>6.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +1009,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>5.5</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,13 +1023,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>3.65</v>
+        <v>6.5</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,13 +1037,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,13 +1051,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>3.36</v>
+        <v>3.1</v>
       </c>
       <c r="D35">
-        <v>77</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,13 +1065,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C36">
-        <v>4.5</v>
+        <v>3.25</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,13 +1079,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,13 +1093,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D38">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,13 +1107,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C39">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,13 +1121,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C40">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,13 +1135,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C41">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,13 +1149,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1121,13 +1163,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>6.75</v>
+        <v>6.5</v>
       </c>
       <c r="D43">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,13 +1177,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C44">
-        <v>3.5</v>
+        <v>3.16</v>
       </c>
       <c r="D44">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,13 +1191,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,13 +1205,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,13 +1219,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C47">
-        <v>4.5</v>
+        <v>3.25</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,13 +1233,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>3.36</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1205,13 +1247,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="D49">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,13 +1261,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C50">
-        <v>3.75</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,13 +1275,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C51">
-        <v>3.25</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,13 +1289,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C52">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,13 +1303,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C53">
-        <v>3.1</v>
+        <v>15</v>
       </c>
       <c r="D53">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,13 +1317,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C54">
-        <v>5.5</v>
+        <v>16</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1289,13 +1331,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C55">
-        <v>3.2</v>
+        <v>6</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,13 +1345,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C56">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="D56">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,13 +1359,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C57">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="D57">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,13 +1373,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C58">
-        <v>3.6</v>
+        <v>6.5</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,10 +1387,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -1359,10 +1401,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1373,13 +1415,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C61">
-        <v>3.16</v>
+        <v>4</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,13 +1429,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>4.5</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,13 +1443,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,13 +1457,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C64">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,16 +1471,21 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <v>6.89</v>
+      </c>
+      <c r="D65">
         <v>3</v>
       </c>
-      <c r="C65">
-        <v>3</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:D65" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D65">
+      <sortCondition ref="B2:B65"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>